<commit_message>
CSS Files switchen Link
</commit_message>
<xml_diff>
--- a/Linksammlung.xlsx
+++ b/Linksammlung.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\GitHub\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Link</t>
   </si>
@@ -111,6 +106,9 @@
   </si>
   <si>
     <t>https://datatables.net/examples/advanced_init/events_live.html</t>
+  </si>
+  <si>
+    <t>http://stackoverflow.com/questions/8796107/how-to-make-changeable-themes-using-css-and-javascript</t>
   </si>
 </sst>
 </file>
@@ -156,7 +154,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -321,6 +319,26 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -329,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -346,9 +364,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -619,7 +639,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -627,11 +647,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -656,163 +676,165 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="9"/>
-      <c r="B3" s="10" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
+      <c r="A4" s="16"/>
+      <c r="B4" s="17" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="10" t="s">
+    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="11"/>
+      <c r="B9" s="12"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B10" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="10" t="s">
+    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="11"/>
-      <c r="B11" s="12"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="5" t="s">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="11"/>
+      <c r="B12" s="12"/>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B12" s="13" t="s">
+      <c r="B13" s="13" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
-      <c r="B13" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="10" t="s">
+    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="11"/>
-      <c r="B25" s="12"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+      <c r="B26" s="12"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B27" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10" t="s">
+    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A28" s="14"/>
-      <c r="B28" s="15"/>
-    </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-      <c r="B29" s="3"/>
+      <c r="A29" s="14"/>
+      <c r="B29" s="15"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
@@ -830,13 +852,17 @@
       <c r="A33" s="1"/>
       <c r="B33" s="3"/>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="2"/>
-      <c r="B34" s="4"/>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="2"/>
+      <c r="B35" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B12" r:id="rId1"/>
+    <hyperlink ref="B13" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>

<commit_message>
Change css code example
</commit_message>
<xml_diff>
--- a/Linksammlung.xlsx
+++ b/Linksammlung.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="L:\GitHub\Documents\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>Link</t>
   </si>
@@ -109,6 +114,9 @@
   </si>
   <si>
     <t>http://stackoverflow.com/questions/8796107/how-to-make-changeable-themes-using-css-and-javascript</t>
+  </si>
+  <si>
+    <t>https://www.thesitewizard.com/javascripts/change-style-sheets.shtml</t>
   </si>
 </sst>
 </file>
@@ -365,10 +373,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -639,7 +647,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -647,11 +655,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -682,163 +690,165 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
       <c r="B4" s="17" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="17" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="9"/>
-      <c r="B8" s="10" t="s">
+    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="11"/>
-      <c r="B9" s="12"/>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B11" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="9"/>
-      <c r="B11" s="10" t="s">
+    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="11"/>
-      <c r="B12" s="12"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="11"/>
+      <c r="B13" s="12"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="13" t="s">
+      <c r="B14" s="13" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
-      <c r="B14" s="3" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="10" t="s">
+    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="10" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="11"/>
-      <c r="B26" s="12"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+      <c r="B27" s="12"/>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B28" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="10" t="s">
+    <row r="29" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" s="14"/>
-      <c r="B29" s="15"/>
-    </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
-      <c r="B30" s="3"/>
+      <c r="A30" s="14"/>
+      <c r="B30" s="15"/>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
@@ -856,15 +866,20 @@
       <c r="A34" s="1"/>
       <c r="B34" s="3"/>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="2"/>
-      <c r="B35" s="4"/>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="2"/>
+      <c r="B36" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B13" r:id="rId1"/>
+    <hyperlink ref="B14" r:id="rId1"/>
+    <hyperlink ref="B4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Test-Datenbank + aktualisierte Linksammlung
Die Datenbank in die das SQL-File importiert werden muss sollte
"editortest" heißen, sonst müsste die Datei config.php ensprechen
geändert werden.
</commit_message>
<xml_diff>
--- a/Linksammlung.xlsx
+++ b/Linksammlung.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Link</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>https://editor.datatables.net/</t>
+  </si>
+  <si>
+    <t>https://editor.datatables.net/download/</t>
+  </si>
+  <si>
+    <t>https://editor.datatables.net/manual/index</t>
+  </si>
+  <si>
+    <t>https://editor.datatables.net/manual/php/installing</t>
+  </si>
+  <si>
+    <t>https://editor.datatables.net/examples/sql/mysql.sql</t>
   </si>
 </sst>
 </file>
@@ -167,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -329,11 +341,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -349,6 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -629,11 +653,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D22" sqref="D22"/>
+      <selection pane="bottomLeft" activeCell="B36" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,54 +844,85 @@
         <v>21</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="B30" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="11"/>
-      <c r="B31" s="12"/>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+      <c r="B31" s="3" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="9"/>
+      <c r="B32" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="B33" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+      <c r="B34" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+      <c r="B35" s="15"/>
+    </row>
+    <row r="36" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="15"/>
+    </row>
+    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="11"/>
+      <c r="B37" s="12"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B38" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A33" s="1"/>
-      <c r="B33" s="3" t="s">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" s="1"/>
-      <c r="B35" s="3"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" s="1"/>
-      <c r="B36" s="3"/>
-    </row>
-    <row r="37" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="2"/>
-      <c r="B37" s="4"/>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="2"/>
+      <c r="B43" s="4"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B32" r:id="rId3" location="/paymentinformation_x000a_"/>
-    <hyperlink ref="B30" r:id="rId4"/>
+    <hyperlink ref="B38" r:id="rId3" location="/paymentinformation_x000a_"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>